<commit_message>
Updated carbon price projection
</commit_message>
<xml_diff>
--- a/InputData/fuels/FoVTStCT/Fraction of Vehicle Types Subject to Carbon Tax.xlsx
+++ b/InputData/fuels/FoVTStCT/Fraction of Vehicle Types Subject to Carbon Tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\fuels\FoVTStCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963B1D52-B69F-40AB-886E-BB5B6893D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81DD04B-BF17-45A0-90BC-D49954BE1126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35835" yWindow="3240" windowWidth="19185" windowHeight="11265" activeTab="4" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
+    <workbookView xWindow="35505" yWindow="2805" windowWidth="21600" windowHeight="12525" activeTab="4" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>Unit: dimensionless</t>
   </si>
@@ -294,6 +294,15 @@
   <si>
     <t>H2 2024 projections</t>
   </si>
+  <si>
+    <t>Near-term projections from Reuters</t>
+  </si>
+  <si>
+    <t>https://www.reuters.com/markets/europe/analysts-expect-eu-carbon-prices-soar-by-2027-2024-10-18/</t>
+  </si>
+  <si>
+    <t>* from Reuters</t>
+  </si>
 </sst>
 </file>
 
@@ -373,7 +382,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,7 +497,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -521,6 +536,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -909,13 +925,13 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.724665391969438</c:v>
+                  <c:v>73.499043977055436</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.262664165103189</c:v>
+                  <c:v>86.754221388367725</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.727440147329659</c:v>
+                  <c:v>102.33885819521178</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>102.31464737793851</c:v>
@@ -1112,7 +1128,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'ETS Projections'!$C$57:$AE$57</c:f>
+              <c:f>'ETS Projections'!$C$62:$AE$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -2074,7 +2090,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>706888</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>105192</xdr:rowOff>
+      <xdr:rowOff>102017</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2865,10 +2881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1D82A8-246A-43A9-9BCA-A1657349D44C}">
-  <dimension ref="A1:AE70"/>
+  <dimension ref="A1:AE75"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4083,14 +4099,17 @@
       <c r="E28">
         <v>65.320000000000007</v>
       </c>
-      <c r="F28">
-        <v>70.840000000000032</v>
-      </c>
-      <c r="G28">
-        <v>85.56</v>
-      </c>
-      <c r="H28">
-        <v>103.96000000000001</v>
+      <c r="F28" s="36">
+        <f>F55</f>
+        <v>76.88</v>
+      </c>
+      <c r="G28" s="36">
+        <f t="shared" ref="G28:H28" si="1">G55</f>
+        <v>92.48</v>
+      </c>
+      <c r="H28" s="36">
+        <f t="shared" si="1"/>
+        <v>111.14</v>
       </c>
       <c r="I28">
         <v>113.16000000000001</v>
@@ -4156,39 +4175,39 @@
         <v>0.9380863039399624</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" ref="H29:P29" si="1">1/(1+SUM($I4:$I5)+$I6*(H27-$F27))</f>
+        <f t="shared" ref="H29:P29" si="2">1/(1+SUM($I4:$I5)+$I6*(H27-$F27))</f>
         <v>0.92081031307550643</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.90415913200723319</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.88809946714031962</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.8726003490401395</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85763293310463129</v>
       </c>
       <c r="M29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.84317032040472184</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.82918739635157546</v>
       </c>
       <c r="O29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81566068515497558</v>
       </c>
       <c r="P29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.8025682182985554</v>
       </c>
       <c r="Q29" s="3"/>
@@ -4216,54 +4235,54 @@
         <v>86.339434799999992</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" ref="D30:P30" si="2">D28*D29</f>
+        <f t="shared" ref="D30:P30" si="3">D28*D29</f>
         <v>85</v>
       </c>
       <c r="E30">
         <v>65</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="2"/>
-        <v>67.724665391969438</v>
+        <f t="shared" si="3"/>
+        <v>73.499043977055436</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="2"/>
-        <v>80.262664165103189</v>
+        <f t="shared" si="3"/>
+        <v>86.754221388367725</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="2"/>
-        <v>95.727440147329659</v>
+        <f t="shared" si="3"/>
+        <v>102.33885819521178</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102.31464737793851</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115.20426287744226</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126.84118673647468</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>133.36052658215647</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>134.58767739188337</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>134.56255154707881</v>
       </c>
       <c r="O30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>138.80097879282221</v>
       </c>
       <c r="P30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>141.7063222183987</v>
       </c>
       <c r="Q30" s="4">
@@ -4271,59 +4290,59 @@
         <v>146.64136826580562</v>
       </c>
       <c r="R30" s="4">
-        <f t="shared" ref="R30:AE30" si="3">R31/$S3</f>
+        <f t="shared" ref="R30:AE30" si="4">R31/$S3</f>
         <v>151.34141212047891</v>
       </c>
       <c r="S30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156.04145597515216</v>
       </c>
       <c r="T30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160.74149982982544</v>
       </c>
       <c r="U30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>165.44154368449873</v>
       </c>
       <c r="V30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170.14158753917195</v>
       </c>
       <c r="W30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>174.84163139384518</v>
       </c>
       <c r="X30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>179.54167524851843</v>
       </c>
       <c r="Y30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>184.24171910319166</v>
       </c>
       <c r="Z30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>189.17676515059858</v>
       </c>
       <c r="AA30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>193.87680900527187</v>
       </c>
       <c r="AB30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>198.57685285994512</v>
       </c>
       <c r="AC30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>203.27689671461837</v>
       </c>
       <c r="AD30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>207.97694056929163</v>
       </c>
       <c r="AE30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>212.67698442396488</v>
       </c>
     </row>
@@ -4336,55 +4355,55 @@
         <v>70.464168387550075</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" ref="D31:P31" si="4">D30*$S3</f>
+        <f t="shared" ref="D31:P31" si="5">D30*$S3</f>
         <v>69.371015999999997</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>53.048423999999997</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="4"/>
-        <v>55.27210407648186</v>
+        <f t="shared" si="5"/>
+        <v>59.98474536137666</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="4"/>
-        <v>65.504735999999994</v>
+        <f t="shared" si="5"/>
+        <v>70.802688000000003</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="4"/>
-        <v>78.125997436464104</v>
+        <f t="shared" si="5"/>
+        <v>83.521771403314915</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83.502012238698015</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>94.021608980461806</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>103.51884699476439</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>108.83947321528473</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>109.84098731476682</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>109.82048136909681</v>
       </c>
       <c r="O31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>113.27958730179448</v>
       </c>
       <c r="P31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>115.65072406957285</v>
       </c>
       <c r="Q31" s="4">
@@ -4392,1480 +4411,1526 @@
         <v>119.67836122622464</v>
       </c>
       <c r="R31" s="4">
-        <f t="shared" ref="R31:AE31" si="5">Q31*R13/Q13</f>
+        <f t="shared" ref="R31:AE31" si="6">Q31*R13/Q13</f>
         <v>123.51420613732159</v>
       </c>
       <c r="S31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>127.35005104841855</v>
       </c>
       <c r="T31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>131.18589595951551</v>
       </c>
       <c r="U31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>135.02174087061246</v>
       </c>
       <c r="V31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>138.85758578170939</v>
       </c>
       <c r="W31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>142.69343069280632</v>
       </c>
       <c r="X31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>146.52927560390324</v>
       </c>
       <c r="Y31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150.36512051500017</v>
       </c>
       <c r="Z31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>154.39275767165196</v>
       </c>
       <c r="AA31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>158.22860258274892</v>
       </c>
       <c r="AB31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>162.06444749384588</v>
       </c>
       <c r="AC31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>165.9002924049428</v>
       </c>
       <c r="AD31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>169.73613731603976</v>
       </c>
       <c r="AE31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>173.57198222713669</v>
       </c>
     </row>
-    <row r="52" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="F32" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <v>2022</v>
+      </c>
+      <c r="D54">
+        <v>2023</v>
+      </c>
+      <c r="E54">
+        <v>2024</v>
+      </c>
+      <c r="F54">
+        <v>2025</v>
+      </c>
+      <c r="G54">
+        <v>2026</v>
+      </c>
+      <c r="H54">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="F55">
+        <v>76.88</v>
+      </c>
+      <c r="G55">
+        <v>92.48</v>
+      </c>
+      <c r="H55">
+        <v>111.14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
         <v>25</v>
       </c>
-      <c r="C55">
+      <c r="C60">
         <v>2022</v>
       </c>
-      <c r="D55">
+      <c r="D60">
         <v>2023</v>
       </c>
-      <c r="E55">
+      <c r="E60">
         <v>2024</v>
       </c>
-      <c r="F55">
+      <c r="F60">
         <v>2025</v>
       </c>
-      <c r="G55">
+      <c r="G60">
         <v>2026</v>
       </c>
-      <c r="H55">
+      <c r="H60">
         <v>2027</v>
       </c>
-      <c r="I55">
+      <c r="I60">
         <v>2028</v>
       </c>
-      <c r="J55">
+      <c r="J60">
         <v>2029</v>
       </c>
-      <c r="K55">
+      <c r="K60">
         <v>2030</v>
       </c>
-      <c r="L55">
+      <c r="L60">
         <v>2031</v>
       </c>
-      <c r="M55">
+      <c r="M60">
         <v>2032</v>
       </c>
-      <c r="N55">
+      <c r="N60">
         <v>2033</v>
       </c>
-      <c r="O55">
+      <c r="O60">
         <v>2034</v>
       </c>
-      <c r="P55">
+      <c r="P60">
         <v>2035</v>
       </c>
-      <c r="Q55">
+      <c r="Q60">
         <v>2036</v>
       </c>
-      <c r="R55">
+      <c r="R60">
         <v>2037</v>
       </c>
-      <c r="S55">
+      <c r="S60">
         <v>2038</v>
       </c>
-      <c r="T55">
+      <c r="T60">
         <v>2039</v>
       </c>
-      <c r="U55">
+      <c r="U60">
         <v>2040</v>
       </c>
-      <c r="V55">
+      <c r="V60">
         <v>2041</v>
       </c>
-      <c r="W55">
+      <c r="W60">
         <v>2042</v>
       </c>
-      <c r="X55">
+      <c r="X60">
         <v>2043</v>
       </c>
-      <c r="Y55">
+      <c r="Y60">
         <v>2044</v>
       </c>
-      <c r="Z55">
+      <c r="Z60">
         <v>2045</v>
       </c>
-      <c r="AA55">
+      <c r="AA60">
         <v>2046</v>
       </c>
-      <c r="AB55">
+      <c r="AB60">
         <v>2047</v>
       </c>
-      <c r="AC55">
+      <c r="AC60">
         <v>2048</v>
       </c>
-      <c r="AD55">
+      <c r="AD60">
         <v>2049</v>
       </c>
-      <c r="AE55">
+      <c r="AE60">
         <v>2050</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
         <v>62</v>
       </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56" s="31">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61" s="31">
         <v>50</v>
       </c>
-      <c r="I56" s="31">
-        <f>H56+25</f>
+      <c r="I61" s="31">
+        <f>H61+25</f>
         <v>75</v>
       </c>
-      <c r="J56" s="31">
-        <f t="shared" ref="J56:U56" si="6">I56+25</f>
+      <c r="J61" s="31">
+        <f t="shared" ref="J61:U61" si="7">I61+25</f>
         <v>100</v>
       </c>
-      <c r="K56" s="31">
-        <f t="shared" si="6"/>
+      <c r="K61" s="31">
+        <f t="shared" si="7"/>
         <v>125</v>
       </c>
-      <c r="L56" s="31">
-        <f t="shared" si="6"/>
+      <c r="L61" s="31">
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
-      <c r="M56" s="31">
-        <f t="shared" si="6"/>
+      <c r="M61" s="31">
+        <f t="shared" si="7"/>
         <v>175</v>
       </c>
-      <c r="N56" s="31">
-        <f t="shared" si="6"/>
+      <c r="N61" s="31">
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
-      <c r="O56" s="31">
-        <f t="shared" si="6"/>
+      <c r="O61" s="31">
+        <f t="shared" si="7"/>
         <v>225</v>
       </c>
-      <c r="P56" s="31">
-        <f t="shared" si="6"/>
+      <c r="P61" s="31">
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
-      <c r="Q56" s="31">
-        <f t="shared" si="6"/>
+      <c r="Q61" s="31">
+        <f t="shared" si="7"/>
         <v>275</v>
       </c>
-      <c r="R56" s="31">
-        <f t="shared" si="6"/>
+      <c r="R61" s="31">
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
-      <c r="S56" s="31">
-        <f t="shared" si="6"/>
+      <c r="S61" s="31">
+        <f t="shared" si="7"/>
         <v>325</v>
       </c>
-      <c r="T56" s="31">
-        <f t="shared" si="6"/>
+      <c r="T61" s="31">
+        <f t="shared" si="7"/>
         <v>350</v>
       </c>
-      <c r="U56" s="31">
-        <f t="shared" si="6"/>
+      <c r="U61" s="31">
+        <f t="shared" si="7"/>
         <v>375</v>
       </c>
-      <c r="V56" s="31">
-        <f>U56+15</f>
+      <c r="V61" s="31">
+        <f>U61+15</f>
         <v>390</v>
       </c>
-      <c r="W56" s="31">
-        <f t="shared" ref="W56:Z56" si="7">V56+15</f>
+      <c r="W61" s="31">
+        <f t="shared" ref="W61:Z61" si="8">V61+15</f>
         <v>405</v>
       </c>
-      <c r="X56" s="31">
-        <f t="shared" si="7"/>
+      <c r="X61" s="31">
+        <f t="shared" si="8"/>
         <v>420</v>
       </c>
-      <c r="Y56" s="31">
-        <f t="shared" si="7"/>
+      <c r="Y61" s="31">
+        <f t="shared" si="8"/>
         <v>435</v>
       </c>
-      <c r="Z56" s="31">
-        <f t="shared" si="7"/>
+      <c r="Z61" s="31">
+        <f t="shared" si="8"/>
         <v>450</v>
       </c>
-      <c r="AA56" s="31">
-        <f>Z56+5</f>
+      <c r="AA61" s="31">
+        <f>Z61+5</f>
         <v>455</v>
       </c>
-      <c r="AB56" s="31">
-        <f t="shared" ref="AB56:AE56" si="8">AA56+5</f>
+      <c r="AB61" s="31">
+        <f t="shared" ref="AB61:AE61" si="9">AA61+5</f>
         <v>460</v>
       </c>
-      <c r="AC56" s="31">
-        <f t="shared" si="8"/>
+      <c r="AC61" s="31">
+        <f t="shared" si="9"/>
         <v>465</v>
       </c>
-      <c r="AD56" s="31">
-        <f t="shared" si="8"/>
+      <c r="AD61" s="31">
+        <f t="shared" si="9"/>
         <v>470</v>
       </c>
-      <c r="AE56" s="31">
-        <f t="shared" si="8"/>
+      <c r="AE61" s="31">
+        <f t="shared" si="9"/>
         <v>475</v>
-      </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57" s="31">
-        <f>H56/(1+0.02)^(H55-$D55)</f>
-        <v>46.192271301325711</v>
-      </c>
-      <c r="I57" s="31">
-        <f t="shared" ref="I57:AD57" si="9">I56/(1+0.02)^(I55-$D55)</f>
-        <v>67.929810737243685</v>
-      </c>
-      <c r="J57" s="31">
-        <f t="shared" si="9"/>
-        <v>88.797138218619196</v>
-      </c>
-      <c r="K57" s="31">
-        <f t="shared" si="9"/>
-        <v>108.82002232673923</v>
-      </c>
-      <c r="L57" s="31">
-        <f t="shared" si="9"/>
-        <v>128.02355567851674</v>
-      </c>
-      <c r="M57" s="31">
-        <f t="shared" si="9"/>
-        <v>146.43217152771521</v>
-      </c>
-      <c r="N57" s="31">
-        <f t="shared" si="9"/>
-        <v>164.06965997503107</v>
-      </c>
-      <c r="O57" s="31">
-        <f t="shared" si="9"/>
-        <v>180.95918379599019</v>
-      </c>
-      <c r="P57" s="31">
-        <f t="shared" si="9"/>
-        <v>197.12329389541409</v>
-      </c>
-      <c r="Q57" s="31">
-        <f t="shared" si="9"/>
-        <v>212.58394439701522</v>
-      </c>
-      <c r="R57" s="31">
-        <f t="shared" si="9"/>
-        <v>227.36250737648683</v>
-      </c>
-      <c r="S57" s="31">
-        <f t="shared" si="9"/>
-        <v>241.47978724626876</v>
-      </c>
-      <c r="T57" s="31">
-        <f t="shared" si="9"/>
-        <v>254.95603479998206</v>
-      </c>
-      <c r="U57" s="31">
-        <f t="shared" si="9"/>
-        <v>267.81096092435087</v>
-      </c>
-      <c r="V57" s="31">
-        <f t="shared" si="9"/>
-        <v>273.06215623659307</v>
-      </c>
-      <c r="W57" s="31">
-        <f t="shared" si="9"/>
-        <v>278.00445770693869</v>
-      </c>
-      <c r="X57" s="31">
-        <f t="shared" si="9"/>
-        <v>282.64795990538425</v>
-      </c>
-      <c r="Y57" s="31">
-        <f t="shared" si="9"/>
-        <v>287.00248029608349</v>
-      </c>
-      <c r="Z57" s="31">
-        <f t="shared" si="9"/>
-        <v>291.07756622320835</v>
-      </c>
-      <c r="AA57" s="31">
-        <f t="shared" si="9"/>
-        <v>288.54094255241796</v>
-      </c>
-      <c r="AB57" s="31">
-        <f t="shared" si="9"/>
-        <v>285.99188445186866</v>
-      </c>
-      <c r="AC57" s="31">
-        <f t="shared" si="9"/>
-        <v>283.43185479564988</v>
-      </c>
-      <c r="AD57" s="31">
-        <f t="shared" si="9"/>
-        <v>280.86226387087379</v>
-      </c>
-      <c r="AE57" s="31">
-        <f>AE56/(1+0.02)^(AE55-$D55)</f>
-        <v>278.28447087748242</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="33">
-        <f>C57*$P$4*$P$5</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="33">
-        <f>D57*$P$4*$P$5</f>
-        <v>0</v>
-      </c>
-      <c r="E58" s="33">
-        <f>E57*$P$4*$P$5</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="33">
-        <f>F57*$P$4*$P$5</f>
-        <v>0</v>
-      </c>
-      <c r="G58" s="33">
-        <f>G57*$P$4*$P$5</f>
-        <v>0</v>
-      </c>
-      <c r="H58" s="33">
-        <f t="shared" ref="H58:AE58" si="10">H57*$S3</f>
-        <v>37.698879900242432</v>
-      </c>
-      <c r="I58" s="33">
-        <f t="shared" si="10"/>
-        <v>55.439529265062397</v>
-      </c>
-      <c r="J58" s="33">
-        <f t="shared" si="10"/>
-        <v>72.469972895506402</v>
-      </c>
-      <c r="K58" s="33">
-        <f t="shared" si="10"/>
-        <v>88.811241293512765</v>
-      </c>
-      <c r="L58" s="33">
-        <f t="shared" si="10"/>
-        <v>104.4838132864856</v>
-      </c>
-      <c r="M58" s="33">
-        <f t="shared" si="10"/>
-        <v>119.5076295760456</v>
-      </c>
-      <c r="N58" s="33">
-        <f t="shared" si="10"/>
-        <v>133.90210596755813</v>
-      </c>
-      <c r="O58" s="33">
-        <f t="shared" si="10"/>
-        <v>147.68614628774796</v>
-      </c>
-      <c r="P58" s="33">
-        <f t="shared" si="10"/>
-        <v>160.87815499754674</v>
-      </c>
-      <c r="Q58" s="33">
-        <f t="shared" si="10"/>
-        <v>173.49604950715826</v>
-      </c>
-      <c r="R58" s="33">
-        <f t="shared" si="10"/>
-        <v>185.55727220016925</v>
-      </c>
-      <c r="S58" s="33">
-        <f t="shared" si="10"/>
-        <v>197.07880217338243</v>
-      </c>
-      <c r="T58" s="33">
-        <f t="shared" si="10"/>
-        <v>208.07716669889544</v>
-      </c>
-      <c r="U58" s="33">
-        <f t="shared" si="10"/>
-        <v>218.5684524148061</v>
-      </c>
-      <c r="V58" s="33">
-        <f t="shared" si="10"/>
-        <v>222.85410834450821</v>
-      </c>
-      <c r="W58" s="33">
-        <f t="shared" si="10"/>
-        <v>226.88766686658079</v>
-      </c>
-      <c r="X58" s="33">
-        <f t="shared" si="10"/>
-        <v>230.6773664583973</v>
-      </c>
-      <c r="Y58" s="33">
-        <f t="shared" si="10"/>
-        <v>234.23121944305049</v>
-      </c>
-      <c r="Z58" s="33">
-        <f t="shared" si="10"/>
-        <v>237.55701769072056</v>
-      </c>
-      <c r="AA58" s="33">
-        <f t="shared" si="10"/>
-        <v>235.48680402892785</v>
-      </c>
-      <c r="AB58" s="33">
-        <f t="shared" si="10"/>
-        <v>233.4064422609498</v>
-      </c>
-      <c r="AC58" s="33">
-        <f t="shared" si="10"/>
-        <v>231.31712628163183</v>
-      </c>
-      <c r="AD58" s="33">
-        <f t="shared" si="10"/>
-        <v>229.22000706803067</v>
-      </c>
-      <c r="AE58" s="33">
-        <f t="shared" si="10"/>
-        <v>227.11619390345138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
-      <c r="Q59" s="9"/>
-      <c r="R59" s="9"/>
-      <c r="S59" s="9"/>
-      <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
-      <c r="V59" s="9"/>
-      <c r="W59" s="9"/>
-      <c r="X59" s="9"/>
-      <c r="Y59" s="9"/>
-      <c r="Z59" s="9"/>
-      <c r="AA59" s="9"/>
-      <c r="AB59" s="9"/>
-      <c r="AC59" s="9"/>
-      <c r="AD59" s="9"/>
-      <c r="AE59" s="9"/>
-    </row>
-    <row r="60" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C62">
-        <v>2022</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>2023</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>2024</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>2025</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>2026</v>
-      </c>
-      <c r="H62">
-        <v>2027</v>
-      </c>
-      <c r="I62">
-        <v>2028</v>
-      </c>
-      <c r="J62">
-        <v>2029</v>
-      </c>
-      <c r="K62">
-        <v>2030</v>
-      </c>
-      <c r="L62">
-        <v>2031</v>
-      </c>
-      <c r="M62">
-        <v>2032</v>
-      </c>
-      <c r="N62">
-        <v>2033</v>
-      </c>
-      <c r="O62">
-        <v>2034</v>
-      </c>
-      <c r="P62">
-        <v>2035</v>
-      </c>
-      <c r="Q62">
-        <v>2036</v>
-      </c>
-      <c r="R62">
-        <v>2037</v>
-      </c>
-      <c r="S62">
-        <v>2038</v>
-      </c>
-      <c r="T62">
-        <v>2039</v>
-      </c>
-      <c r="U62">
-        <v>2040</v>
-      </c>
-      <c r="V62">
-        <v>2041</v>
-      </c>
-      <c r="W62">
-        <v>2042</v>
-      </c>
-      <c r="X62">
-        <v>2043</v>
-      </c>
-      <c r="Y62">
-        <v>2044</v>
-      </c>
-      <c r="Z62">
-        <v>2045</v>
-      </c>
-      <c r="AA62">
-        <v>2046</v>
-      </c>
-      <c r="AB62">
-        <v>2047</v>
-      </c>
-      <c r="AC62">
-        <v>2048</v>
-      </c>
-      <c r="AD62">
-        <v>2049</v>
-      </c>
-      <c r="AE62">
-        <v>2050</v>
+        <v>0</v>
+      </c>
+      <c r="H62" s="31">
+        <f>H61/(1+0.02)^(H60-$D60)</f>
+        <v>46.192271301325711</v>
+      </c>
+      <c r="I62" s="31">
+        <f t="shared" ref="I62:AD62" si="10">I61/(1+0.02)^(I60-$D60)</f>
+        <v>67.929810737243685</v>
+      </c>
+      <c r="J62" s="31">
+        <f t="shared" si="10"/>
+        <v>88.797138218619196</v>
+      </c>
+      <c r="K62" s="31">
+        <f t="shared" si="10"/>
+        <v>108.82002232673923</v>
+      </c>
+      <c r="L62" s="31">
+        <f t="shared" si="10"/>
+        <v>128.02355567851674</v>
+      </c>
+      <c r="M62" s="31">
+        <f t="shared" si="10"/>
+        <v>146.43217152771521</v>
+      </c>
+      <c r="N62" s="31">
+        <f t="shared" si="10"/>
+        <v>164.06965997503107</v>
+      </c>
+      <c r="O62" s="31">
+        <f t="shared" si="10"/>
+        <v>180.95918379599019</v>
+      </c>
+      <c r="P62" s="31">
+        <f t="shared" si="10"/>
+        <v>197.12329389541409</v>
+      </c>
+      <c r="Q62" s="31">
+        <f t="shared" si="10"/>
+        <v>212.58394439701522</v>
+      </c>
+      <c r="R62" s="31">
+        <f t="shared" si="10"/>
+        <v>227.36250737648683</v>
+      </c>
+      <c r="S62" s="31">
+        <f t="shared" si="10"/>
+        <v>241.47978724626876</v>
+      </c>
+      <c r="T62" s="31">
+        <f t="shared" si="10"/>
+        <v>254.95603479998206</v>
+      </c>
+      <c r="U62" s="31">
+        <f t="shared" si="10"/>
+        <v>267.81096092435087</v>
+      </c>
+      <c r="V62" s="31">
+        <f t="shared" si="10"/>
+        <v>273.06215623659307</v>
+      </c>
+      <c r="W62" s="31">
+        <f t="shared" si="10"/>
+        <v>278.00445770693869</v>
+      </c>
+      <c r="X62" s="31">
+        <f t="shared" si="10"/>
+        <v>282.64795990538425</v>
+      </c>
+      <c r="Y62" s="31">
+        <f t="shared" si="10"/>
+        <v>287.00248029608349</v>
+      </c>
+      <c r="Z62" s="31">
+        <f t="shared" si="10"/>
+        <v>291.07756622320835</v>
+      </c>
+      <c r="AA62" s="31">
+        <f t="shared" si="10"/>
+        <v>288.54094255241796</v>
+      </c>
+      <c r="AB62" s="31">
+        <f t="shared" si="10"/>
+        <v>285.99188445186866</v>
+      </c>
+      <c r="AC62" s="31">
+        <f t="shared" si="10"/>
+        <v>283.43185479564988</v>
+      </c>
+      <c r="AD62" s="31">
+        <f t="shared" si="10"/>
+        <v>280.86226387087379</v>
+      </c>
+      <c r="AE62" s="31">
+        <f>AE61/(1+0.02)^(AE60-$D60)</f>
+        <v>278.28447087748242</v>
       </c>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="33">
+        <f>C62*$P$4*$P$5</f>
+        <v>0</v>
+      </c>
+      <c r="D63" s="33">
+        <f>D62*$P$4*$P$5</f>
+        <v>0</v>
+      </c>
+      <c r="E63" s="33">
+        <f>E62*$P$4*$P$5</f>
+        <v>0</v>
+      </c>
+      <c r="F63" s="33">
+        <f>F62*$P$4*$P$5</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="33">
+        <f>G62*$P$4*$P$5</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="33">
+        <f t="shared" ref="H63:AE63" si="11">H62*$S3</f>
+        <v>37.698879900242432</v>
+      </c>
+      <c r="I63" s="33">
+        <f t="shared" si="11"/>
+        <v>55.439529265062397</v>
+      </c>
+      <c r="J63" s="33">
+        <f t="shared" si="11"/>
+        <v>72.469972895506402</v>
+      </c>
+      <c r="K63" s="33">
+        <f t="shared" si="11"/>
+        <v>88.811241293512765</v>
+      </c>
+      <c r="L63" s="33">
+        <f t="shared" si="11"/>
+        <v>104.4838132864856</v>
+      </c>
+      <c r="M63" s="33">
+        <f t="shared" si="11"/>
+        <v>119.5076295760456</v>
+      </c>
+      <c r="N63" s="33">
+        <f t="shared" si="11"/>
+        <v>133.90210596755813</v>
+      </c>
+      <c r="O63" s="33">
+        <f t="shared" si="11"/>
+        <v>147.68614628774796</v>
+      </c>
+      <c r="P63" s="33">
+        <f t="shared" si="11"/>
+        <v>160.87815499754674</v>
+      </c>
+      <c r="Q63" s="33">
+        <f t="shared" si="11"/>
+        <v>173.49604950715826</v>
+      </c>
+      <c r="R63" s="33">
+        <f t="shared" si="11"/>
+        <v>185.55727220016925</v>
+      </c>
+      <c r="S63" s="33">
+        <f t="shared" si="11"/>
+        <v>197.07880217338243</v>
+      </c>
+      <c r="T63" s="33">
+        <f t="shared" si="11"/>
+        <v>208.07716669889544</v>
+      </c>
+      <c r="U63" s="33">
+        <f t="shared" si="11"/>
+        <v>218.5684524148061</v>
+      </c>
+      <c r="V63" s="33">
+        <f t="shared" si="11"/>
+        <v>222.85410834450821</v>
+      </c>
+      <c r="W63" s="33">
+        <f t="shared" si="11"/>
+        <v>226.88766686658079</v>
+      </c>
+      <c r="X63" s="33">
+        <f t="shared" si="11"/>
+        <v>230.6773664583973</v>
+      </c>
+      <c r="Y63" s="33">
+        <f t="shared" si="11"/>
+        <v>234.23121944305049</v>
+      </c>
+      <c r="Z63" s="33">
+        <f t="shared" si="11"/>
+        <v>237.55701769072056</v>
+      </c>
+      <c r="AA63" s="33">
+        <f t="shared" si="11"/>
+        <v>235.48680402892785</v>
+      </c>
+      <c r="AB63" s="33">
+        <f t="shared" si="11"/>
+        <v>233.4064422609498</v>
+      </c>
+      <c r="AC63" s="33">
+        <f t="shared" si="11"/>
+        <v>231.31712628163183</v>
+      </c>
+      <c r="AD63" s="33">
+        <f t="shared" si="11"/>
+        <v>229.22000706803067</v>
+      </c>
+      <c r="AE63" s="33">
+        <f t="shared" si="11"/>
+        <v>227.11619390345138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="9"/>
+      <c r="S64" s="9"/>
+      <c r="T64" s="9"/>
+      <c r="U64" s="9"/>
+      <c r="V64" s="9"/>
+      <c r="W64" s="9"/>
+      <c r="X64" s="9"/>
+      <c r="Y64" s="9"/>
+      <c r="Z64" s="9"/>
+      <c r="AA64" s="9"/>
+      <c r="AB64" s="9"/>
+      <c r="AC64" s="9"/>
+      <c r="AD64" s="9"/>
+      <c r="AE64" s="9"/>
+    </row>
+    <row r="65" spans="1:31" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>2022</v>
+      </c>
+      <c r="D67">
+        <v>2023</v>
+      </c>
+      <c r="E67">
+        <v>2024</v>
+      </c>
+      <c r="F67">
+        <v>2025</v>
+      </c>
+      <c r="G67">
+        <v>2026</v>
+      </c>
+      <c r="H67">
+        <v>2027</v>
+      </c>
+      <c r="I67">
+        <v>2028</v>
+      </c>
+      <c r="J67">
+        <v>2029</v>
+      </c>
+      <c r="K67">
+        <v>2030</v>
+      </c>
+      <c r="L67">
+        <v>2031</v>
+      </c>
+      <c r="M67">
+        <v>2032</v>
+      </c>
+      <c r="N67">
+        <v>2033</v>
+      </c>
+      <c r="O67">
+        <v>2034</v>
+      </c>
+      <c r="P67">
+        <v>2035</v>
+      </c>
+      <c r="Q67">
+        <v>2036</v>
+      </c>
+      <c r="R67">
+        <v>2037</v>
+      </c>
+      <c r="S67">
+        <v>2038</v>
+      </c>
+      <c r="T67">
+        <v>2039</v>
+      </c>
+      <c r="U67">
+        <v>2040</v>
+      </c>
+      <c r="V67">
+        <v>2041</v>
+      </c>
+      <c r="W67">
+        <v>2042</v>
+      </c>
+      <c r="X67">
+        <v>2043</v>
+      </c>
+      <c r="Y67">
+        <v>2044</v>
+      </c>
+      <c r="Z67">
+        <v>2045</v>
+      </c>
+      <c r="AA67">
+        <v>2046</v>
+      </c>
+      <c r="AB67">
+        <v>2047</v>
+      </c>
+      <c r="AC67">
+        <v>2048</v>
+      </c>
+      <c r="AD67">
+        <v>2049</v>
+      </c>
+      <c r="AE67">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="29">
-        <f t="shared" ref="C63:AE63" si="11">C22</f>
+      <c r="C68" s="29">
+        <f t="shared" ref="C68:AE68" si="12">C22</f>
         <v>43.130404778848849</v>
       </c>
-      <c r="D63" s="29">
-        <f t="shared" si="11"/>
+      <c r="D68" s="29">
+        <f t="shared" si="12"/>
         <v>43.130404778848849</v>
       </c>
-      <c r="E63" s="29">
-        <f t="shared" si="11"/>
+      <c r="E68" s="29">
+        <f t="shared" si="12"/>
         <v>43.130404778848849</v>
       </c>
-      <c r="F63" s="29">
-        <f t="shared" si="11"/>
+      <c r="F68" s="29">
+        <f t="shared" si="12"/>
         <v>43.130404778848849</v>
       </c>
-      <c r="G63" s="29">
-        <f t="shared" si="11"/>
+      <c r="G68" s="29">
+        <f t="shared" si="12"/>
         <v>46.806291549773469</v>
       </c>
-      <c r="H63" s="29">
-        <f t="shared" si="11"/>
+      <c r="H68" s="29">
+        <f t="shared" si="12"/>
         <v>50.48217832069809</v>
       </c>
-      <c r="I63" s="29">
-        <f t="shared" si="11"/>
+      <c r="I68" s="29">
+        <f t="shared" si="12"/>
         <v>54.280594650653519</v>
       </c>
-      <c r="J63" s="29">
-        <f t="shared" si="11"/>
+      <c r="J68" s="29">
+        <f t="shared" si="12"/>
         <v>57.95648142157814</v>
       </c>
-      <c r="K63" s="29">
-        <f t="shared" si="11"/>
+      <c r="K68" s="29">
+        <f t="shared" si="12"/>
         <v>61.632368192502753</v>
       </c>
-      <c r="L63" s="29">
-        <f t="shared" si="11"/>
+      <c r="L68" s="29">
+        <f t="shared" si="12"/>
         <v>64.082959373119166</v>
       </c>
-      <c r="M63" s="29">
-        <f t="shared" si="11"/>
+      <c r="M68" s="29">
+        <f t="shared" si="12"/>
         <v>66.53355055373558</v>
       </c>
-      <c r="N63" s="29">
-        <f t="shared" si="11"/>
+      <c r="N68" s="29">
+        <f t="shared" si="12"/>
         <v>68.984141734351994</v>
       </c>
-      <c r="O63" s="29">
-        <f t="shared" si="11"/>
+      <c r="O68" s="29">
+        <f t="shared" si="12"/>
         <v>71.434732914968407</v>
       </c>
-      <c r="P63" s="29">
-        <f t="shared" si="11"/>
+      <c r="P68" s="29">
+        <f t="shared" si="12"/>
         <v>73.885324095584821</v>
       </c>
-      <c r="Q63" s="29">
-        <f t="shared" si="11"/>
+      <c r="Q68" s="29">
+        <f t="shared" si="12"/>
         <v>76.458444835232044</v>
       </c>
-      <c r="R63" s="29">
-        <f t="shared" si="11"/>
+      <c r="R68" s="29">
+        <f t="shared" si="12"/>
         <v>78.909036015848471</v>
       </c>
-      <c r="S63" s="29">
-        <f t="shared" si="11"/>
+      <c r="S68" s="29">
+        <f t="shared" si="12"/>
         <v>81.359627196464885</v>
       </c>
-      <c r="T63" s="29">
-        <f t="shared" si="11"/>
+      <c r="T68" s="29">
+        <f t="shared" si="12"/>
         <v>83.810218377081299</v>
       </c>
-      <c r="U63" s="29">
-        <f t="shared" si="11"/>
+      <c r="U68" s="29">
+        <f t="shared" si="12"/>
         <v>86.260809557697698</v>
       </c>
-      <c r="V63" s="29">
-        <f t="shared" si="11"/>
+      <c r="V68" s="29">
+        <f t="shared" si="12"/>
         <v>88.711400738314111</v>
       </c>
-      <c r="W63" s="29">
-        <f t="shared" si="11"/>
+      <c r="W68" s="29">
+        <f t="shared" si="12"/>
         <v>91.161991918930525</v>
       </c>
-      <c r="X63" s="29">
-        <f t="shared" si="11"/>
+      <c r="X68" s="29">
+        <f t="shared" si="12"/>
         <v>93.612583099546939</v>
       </c>
-      <c r="Y63" s="29">
-        <f t="shared" si="11"/>
+      <c r="Y68" s="29">
+        <f t="shared" si="12"/>
         <v>96.063174280163352</v>
       </c>
-      <c r="Z63" s="29">
-        <f t="shared" si="11"/>
+      <c r="Z68" s="29">
+        <f t="shared" si="12"/>
         <v>98.636295019810575</v>
       </c>
-      <c r="AA63" s="29">
-        <f t="shared" si="11"/>
+      <c r="AA68" s="29">
+        <f t="shared" si="12"/>
         <v>101.08688620042699</v>
       </c>
-      <c r="AB63" s="29">
-        <f t="shared" si="11"/>
+      <c r="AB68" s="29">
+        <f t="shared" si="12"/>
         <v>103.5374773810434</v>
       </c>
-      <c r="AC63" s="29">
-        <f t="shared" si="11"/>
+      <c r="AC68" s="29">
+        <f t="shared" si="12"/>
         <v>105.98806856165982</v>
       </c>
-      <c r="AD63" s="29">
-        <f t="shared" si="11"/>
+      <c r="AD68" s="29">
+        <f t="shared" si="12"/>
         <v>108.43865974227623</v>
       </c>
-      <c r="AE63" s="29">
-        <f t="shared" si="11"/>
+      <c r="AE68" s="29">
+        <f t="shared" si="12"/>
         <v>110.88925092289264</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="34">
-        <f t="shared" ref="C64:AE64" si="12">MAX(C57,C30)</f>
+      <c r="C69" s="34">
+        <f t="shared" ref="C69:AE69" si="13">MAX(C62,C30)</f>
         <v>86.339434799999992</v>
       </c>
-      <c r="D64" s="34">
-        <f t="shared" si="12"/>
+      <c r="D69" s="34">
+        <f t="shared" si="13"/>
         <v>85</v>
       </c>
-      <c r="E64" s="34">
-        <f t="shared" si="12"/>
+      <c r="E69" s="34">
+        <f t="shared" si="13"/>
         <v>65</v>
       </c>
-      <c r="F64" s="34">
-        <f t="shared" si="12"/>
-        <v>67.724665391969438</v>
-      </c>
-      <c r="G64" s="34">
-        <f t="shared" si="12"/>
-        <v>80.262664165103189</v>
-      </c>
-      <c r="H64" s="34">
-        <f>MAX(H57,H30)</f>
-        <v>95.727440147329659</v>
-      </c>
-      <c r="I64" s="34">
-        <f t="shared" si="12"/>
+      <c r="F69" s="34">
+        <f t="shared" si="13"/>
+        <v>73.499043977055436</v>
+      </c>
+      <c r="G69" s="34">
+        <f t="shared" si="13"/>
+        <v>86.754221388367725</v>
+      </c>
+      <c r="H69" s="34">
+        <f>MAX(H62,H30)</f>
+        <v>102.33885819521178</v>
+      </c>
+      <c r="I69" s="34">
+        <f t="shared" si="13"/>
         <v>102.31464737793851</v>
       </c>
-      <c r="J64" s="34">
-        <f t="shared" si="12"/>
+      <c r="J69" s="34">
+        <f t="shared" si="13"/>
         <v>115.20426287744226</v>
       </c>
-      <c r="K64" s="34">
-        <f t="shared" si="12"/>
+      <c r="K69" s="34">
+        <f t="shared" si="13"/>
         <v>126.84118673647468</v>
       </c>
-      <c r="L64" s="34">
-        <f t="shared" si="12"/>
+      <c r="L69" s="34">
+        <f t="shared" si="13"/>
         <v>133.36052658215647</v>
       </c>
-      <c r="M64" s="34">
-        <f t="shared" si="12"/>
+      <c r="M69" s="34">
+        <f t="shared" si="13"/>
         <v>146.43217152771521</v>
       </c>
-      <c r="N64" s="34">
-        <f t="shared" si="12"/>
+      <c r="N69" s="34">
+        <f t="shared" si="13"/>
         <v>164.06965997503107</v>
       </c>
-      <c r="O64" s="34">
-        <f t="shared" si="12"/>
+      <c r="O69" s="34">
+        <f t="shared" si="13"/>
         <v>180.95918379599019</v>
       </c>
-      <c r="P64" s="34">
-        <f t="shared" si="12"/>
+      <c r="P69" s="34">
+        <f t="shared" si="13"/>
         <v>197.12329389541409</v>
       </c>
-      <c r="Q64" s="34">
-        <f t="shared" si="12"/>
+      <c r="Q69" s="34">
+        <f t="shared" si="13"/>
         <v>212.58394439701522</v>
       </c>
-      <c r="R64" s="34">
-        <f t="shared" si="12"/>
+      <c r="R69" s="34">
+        <f t="shared" si="13"/>
         <v>227.36250737648683</v>
       </c>
-      <c r="S64" s="34">
-        <f t="shared" si="12"/>
+      <c r="S69" s="34">
+        <f t="shared" si="13"/>
         <v>241.47978724626876</v>
       </c>
-      <c r="T64" s="34">
-        <f t="shared" si="12"/>
+      <c r="T69" s="34">
+        <f t="shared" si="13"/>
         <v>254.95603479998206</v>
       </c>
-      <c r="U64" s="34">
-        <f t="shared" si="12"/>
+      <c r="U69" s="34">
+        <f t="shared" si="13"/>
         <v>267.81096092435087</v>
       </c>
-      <c r="V64" s="34">
-        <f t="shared" si="12"/>
+      <c r="V69" s="34">
+        <f t="shared" si="13"/>
         <v>273.06215623659307</v>
       </c>
-      <c r="W64" s="34">
-        <f t="shared" si="12"/>
+      <c r="W69" s="34">
+        <f t="shared" si="13"/>
         <v>278.00445770693869</v>
       </c>
-      <c r="X64" s="34">
-        <f t="shared" si="12"/>
+      <c r="X69" s="34">
+        <f t="shared" si="13"/>
         <v>282.64795990538425</v>
       </c>
-      <c r="Y64" s="34">
-        <f t="shared" si="12"/>
+      <c r="Y69" s="34">
+        <f t="shared" si="13"/>
         <v>287.00248029608349</v>
       </c>
-      <c r="Z64" s="34">
-        <f t="shared" si="12"/>
+      <c r="Z69" s="34">
+        <f t="shared" si="13"/>
         <v>291.07756622320835</v>
       </c>
-      <c r="AA64" s="34">
-        <f t="shared" si="12"/>
+      <c r="AA69" s="34">
+        <f t="shared" si="13"/>
         <v>288.54094255241796</v>
       </c>
-      <c r="AB64" s="34">
-        <f t="shared" si="12"/>
+      <c r="AB69" s="34">
+        <f t="shared" si="13"/>
         <v>285.99188445186866</v>
       </c>
-      <c r="AC64" s="34">
-        <f t="shared" si="12"/>
+      <c r="AC69" s="34">
+        <f t="shared" si="13"/>
         <v>283.43185479564988</v>
       </c>
-      <c r="AD64" s="34">
-        <f t="shared" si="12"/>
+      <c r="AD69" s="34">
+        <f t="shared" si="13"/>
         <v>280.86226387087379</v>
       </c>
-      <c r="AE64" s="34">
-        <f t="shared" si="12"/>
+      <c r="AE69" s="34">
+        <f t="shared" si="13"/>
         <v>278.28447087748242</v>
       </c>
     </row>
-    <row r="65" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
         <v>32</v>
       </c>
-      <c r="C65">
-        <f t="shared" ref="C65:AE65" si="13">C30/C64</f>
-        <v>1</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="E65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="G65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="H65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="J65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="K65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="M65" s="35">
-        <f>M30/M64</f>
+      <c r="C70">
+        <f t="shared" ref="C70:AE70" si="14">C30/C69</f>
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M70" s="35">
+        <f>M30/M69</f>
         <v>0.91911276045243906</v>
       </c>
-      <c r="N65">
-        <f t="shared" si="13"/>
+      <c r="N70">
+        <f t="shared" si="14"/>
         <v>0.82015499738072961</v>
       </c>
-      <c r="O65">
-        <f t="shared" si="13"/>
+      <c r="O70">
+        <f t="shared" si="14"/>
         <v>0.76702920449344913</v>
       </c>
-      <c r="P65">
-        <f t="shared" si="13"/>
+      <c r="P70">
+        <f t="shared" si="14"/>
         <v>0.71887152156448098</v>
       </c>
-      <c r="Q65" s="35">
-        <f t="shared" si="13"/>
+      <c r="Q70" s="35">
+        <f t="shared" si="14"/>
         <v>0.68980453195441105</v>
       </c>
-      <c r="R65">
-        <f t="shared" si="13"/>
+      <c r="R70">
+        <f t="shared" si="14"/>
         <v>0.66563926421639297</v>
       </c>
-      <c r="S65">
-        <f t="shared" si="13"/>
+      <c r="S70">
+        <f t="shared" si="14"/>
         <v>0.64618847711678717</v>
       </c>
-      <c r="T65">
-        <f t="shared" si="13"/>
+      <c r="T70">
+        <f t="shared" si="14"/>
         <v>0.6304675233748841</v>
       </c>
-      <c r="U65">
-        <f t="shared" si="13"/>
+      <c r="U70">
+        <f t="shared" si="14"/>
         <v>0.61775493845911467</v>
       </c>
-      <c r="V65">
-        <f t="shared" si="13"/>
+      <c r="V70">
+        <f t="shared" si="14"/>
         <v>0.62308739476792896</v>
       </c>
-      <c r="W65">
-        <f t="shared" si="13"/>
+      <c r="W70">
+        <f t="shared" si="14"/>
         <v>0.62891664700627326</v>
       </c>
-      <c r="X65">
-        <f t="shared" si="13"/>
+      <c r="X70">
+        <f t="shared" si="14"/>
         <v>0.63521305905982683</v>
       </c>
-      <c r="Y65">
-        <f t="shared" si="13"/>
+      <c r="Y70">
+        <f t="shared" si="14"/>
         <v>0.641951661578396</v>
       </c>
-      <c r="Z65">
-        <f t="shared" si="13"/>
+      <c r="Z70">
+        <f t="shared" si="14"/>
         <v>0.64991874023548524</v>
       </c>
-      <c r="AA65">
-        <f t="shared" si="13"/>
+      <c r="AA70">
+        <f t="shared" si="14"/>
         <v>0.6719213131081081</v>
       </c>
-      <c r="AB65">
-        <f t="shared" si="13"/>
+      <c r="AB70">
+        <f t="shared" si="14"/>
         <v>0.69434436309455783</v>
       </c>
-      <c r="AC65">
-        <f t="shared" si="13"/>
+      <c r="AC70">
+        <f t="shared" si="14"/>
         <v>0.71719848448643142</v>
       </c>
-      <c r="AD65">
-        <f t="shared" si="13"/>
+      <c r="AD70">
+        <f t="shared" si="14"/>
         <v>0.74049442492889994</v>
       </c>
-      <c r="AE65">
-        <f t="shared" si="13"/>
+      <c r="AE70">
+        <f t="shared" si="14"/>
         <v>0.76424309180226624</v>
       </c>
     </row>
-    <row r="66" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
         <v>33</v>
       </c>
-      <c r="C66">
-        <f t="shared" ref="C66:AE66" si="14">C57/C64</f>
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <f>H57/H64</f>
-        <v>0.4825395020511708</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="14"/>
+      <c r="C71">
+        <f t="shared" ref="C71:AE71" si="15">C62/C69</f>
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <f>H62/H69</f>
+        <v>0.45136590456397085</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="15"/>
         <v>0.66393045842516363</v>
       </c>
-      <c r="J66">
-        <f t="shared" si="14"/>
+      <c r="J71">
+        <f t="shared" si="15"/>
         <v>0.77077996942773064</v>
       </c>
-      <c r="K66">
-        <f t="shared" si="14"/>
+      <c r="K71">
+        <f t="shared" si="15"/>
         <v>0.85792340111752319</v>
       </c>
-      <c r="L66">
-        <f t="shared" si="14"/>
+      <c r="L71">
+        <f t="shared" si="15"/>
         <v>0.95998088009684113</v>
       </c>
-      <c r="M66">
-        <f>M57/M64</f>
-        <v>1</v>
-      </c>
-      <c r="N66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="O66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="P66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Q66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="R66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="S66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="T66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="U66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="V66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="W66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="X66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Y66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Z66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AA66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AB66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AC66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AD66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AE66">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
+      <c r="M71">
+        <f>M62/M69</f>
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="U71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="V71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="W71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="X71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Y71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Z71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AA71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AB71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AC71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AD71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AE71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="29">
-        <f>C64-C63</f>
+      <c r="C73" s="29">
+        <f>C69-C68</f>
         <v>43.209030021151143</v>
       </c>
-      <c r="D68" s="29">
-        <f t="shared" ref="D68:AE68" si="15">D64-D63</f>
+      <c r="D73" s="29">
+        <f t="shared" ref="D73:AE73" si="16">D69-D68</f>
         <v>41.869595221151151</v>
       </c>
-      <c r="E68" s="29">
-        <f t="shared" si="15"/>
+      <c r="E73" s="29">
+        <f t="shared" si="16"/>
         <v>21.869595221151151</v>
       </c>
-      <c r="F68" s="29">
-        <f t="shared" si="15"/>
-        <v>24.594260613120589</v>
-      </c>
-      <c r="G68" s="29">
-        <f t="shared" si="15"/>
-        <v>33.45637261532972</v>
-      </c>
-      <c r="H68" s="29">
-        <f t="shared" si="15"/>
-        <v>45.24526182663157</v>
-      </c>
-      <c r="I68" s="29">
-        <f t="shared" si="15"/>
+      <c r="F73" s="29">
+        <f t="shared" si="16"/>
+        <v>30.368639198206587</v>
+      </c>
+      <c r="G73" s="29">
+        <f t="shared" si="16"/>
+        <v>39.947929838594256</v>
+      </c>
+      <c r="H73" s="29">
+        <f t="shared" si="16"/>
+        <v>51.856679874513695</v>
+      </c>
+      <c r="I73" s="29">
+        <f t="shared" si="16"/>
         <v>48.034052727284994</v>
       </c>
-      <c r="J68" s="29">
-        <f t="shared" si="15"/>
+      <c r="J73" s="29">
+        <f t="shared" si="16"/>
         <v>57.247781455864121</v>
       </c>
-      <c r="K68" s="29">
-        <f t="shared" si="15"/>
+      <c r="K73" s="29">
+        <f t="shared" si="16"/>
         <v>65.20881854397193</v>
       </c>
-      <c r="L68" s="29">
-        <f t="shared" si="15"/>
+      <c r="L73" s="29">
+        <f t="shared" si="16"/>
         <v>69.277567209037301</v>
       </c>
-      <c r="M68" s="29">
-        <f t="shared" si="15"/>
+      <c r="M73" s="29">
+        <f t="shared" si="16"/>
         <v>79.898620973979632</v>
       </c>
-      <c r="N68" s="29">
-        <f t="shared" si="15"/>
+      <c r="N73" s="29">
+        <f t="shared" si="16"/>
         <v>95.085518240679079</v>
       </c>
-      <c r="O68" s="29">
-        <f t="shared" si="15"/>
+      <c r="O73" s="29">
+        <f t="shared" si="16"/>
         <v>109.52445088102178</v>
       </c>
-      <c r="P68" s="29">
-        <f t="shared" si="15"/>
+      <c r="P73" s="29">
+        <f t="shared" si="16"/>
         <v>123.23796979982927</v>
       </c>
-      <c r="Q68" s="29">
-        <f t="shared" si="15"/>
+      <c r="Q73" s="29">
+        <f t="shared" si="16"/>
         <v>136.12549956178316</v>
       </c>
-      <c r="R68" s="29">
-        <f t="shared" si="15"/>
+      <c r="R73" s="29">
+        <f t="shared" si="16"/>
         <v>148.45347136063836</v>
       </c>
-      <c r="S68" s="29">
-        <f t="shared" si="15"/>
+      <c r="S73" s="29">
+        <f t="shared" si="16"/>
         <v>160.12016004980387</v>
       </c>
-      <c r="T68" s="29">
-        <f t="shared" si="15"/>
+      <c r="T73" s="29">
+        <f t="shared" si="16"/>
         <v>171.14581642290077</v>
       </c>
-      <c r="U68" s="29">
-        <f t="shared" si="15"/>
+      <c r="U73" s="29">
+        <f t="shared" si="16"/>
         <v>181.55015136665315</v>
       </c>
-      <c r="V68" s="29">
-        <f t="shared" si="15"/>
+      <c r="V73" s="29">
+        <f t="shared" si="16"/>
         <v>184.35075549827894</v>
       </c>
-      <c r="W68" s="29">
-        <f t="shared" si="15"/>
+      <c r="W73" s="29">
+        <f t="shared" si="16"/>
         <v>186.84246578800816</v>
       </c>
-      <c r="X68" s="29">
-        <f t="shared" si="15"/>
+      <c r="X73" s="29">
+        <f t="shared" si="16"/>
         <v>189.0353768058373</v>
       </c>
-      <c r="Y68" s="29">
-        <f t="shared" si="15"/>
+      <c r="Y73" s="29">
+        <f t="shared" si="16"/>
         <v>190.93930601592012</v>
       </c>
-      <c r="Z68" s="29">
-        <f t="shared" si="15"/>
+      <c r="Z73" s="29">
+        <f t="shared" si="16"/>
         <v>192.44127120339778</v>
       </c>
-      <c r="AA68" s="29">
-        <f t="shared" si="15"/>
+      <c r="AA73" s="29">
+        <f t="shared" si="16"/>
         <v>187.45405635199097</v>
       </c>
-      <c r="AB68" s="29">
-        <f t="shared" si="15"/>
+      <c r="AB73" s="29">
+        <f t="shared" si="16"/>
         <v>182.45440707082525</v>
       </c>
-      <c r="AC68" s="29">
-        <f t="shared" si="15"/>
+      <c r="AC73" s="29">
+        <f t="shared" si="16"/>
         <v>177.44378623399007</v>
       </c>
-      <c r="AD68" s="29">
-        <f t="shared" si="15"/>
+      <c r="AD73" s="29">
+        <f t="shared" si="16"/>
         <v>172.42360412859756</v>
       </c>
-      <c r="AE68" s="29">
-        <f t="shared" si="15"/>
+      <c r="AE73" s="29">
+        <f t="shared" si="16"/>
         <v>167.39521995458978</v>
       </c>
     </row>
-    <row r="69" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="B69" t="s">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
         <v>65</v>
       </c>
-      <c r="C69">
+      <c r="C74">
         <f>C31/MAX($C31:$AE31)</f>
         <v>0.40596510729099416</v>
       </c>
-      <c r="D69">
-        <f t="shared" ref="D69:AE69" si="16">D31/MAX($C31:$AE31)</f>
+      <c r="D74">
+        <f t="shared" ref="D74:AE74" si="17">D31/MAX($C31:$AE31)</f>
         <v>0.39966713008566629</v>
       </c>
-      <c r="E69">
-        <f t="shared" si="16"/>
+      <c r="E74">
+        <f t="shared" si="17"/>
         <v>0.30562780535962719</v>
       </c>
-      <c r="F69">
-        <f t="shared" si="16"/>
-        <v>0.3184390900378879</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="16"/>
-        <v>0.37739233693995816</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="16"/>
-        <v>0.45010719146036049</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="16"/>
+      <c r="F74">
+        <f t="shared" si="17"/>
+        <v>0.34559002318058735</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="17"/>
+        <v>0.40791541982477014</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="17"/>
+        <v>0.48119385589557961</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="17"/>
         <v>0.48108001745020745</v>
       </c>
-      <c r="J69">
-        <f t="shared" si="16"/>
+      <c r="J74">
+        <f t="shared" si="17"/>
         <v>0.54168655432778845</v>
       </c>
-      <c r="K69">
-        <f t="shared" si="16"/>
+      <c r="K74">
+        <f t="shared" si="17"/>
         <v>0.59640297740737558</v>
       </c>
-      <c r="L69">
-        <f t="shared" si="16"/>
+      <c r="L74">
+        <f t="shared" si="17"/>
         <v>0.62705669324474933</v>
       </c>
-      <c r="M69">
-        <f t="shared" si="16"/>
+      <c r="M74">
+        <f t="shared" si="17"/>
         <v>0.63282671491893583</v>
       </c>
-      <c r="N69">
-        <f t="shared" si="16"/>
+      <c r="N74">
+        <f t="shared" si="17"/>
         <v>0.63270857404500624</v>
       </c>
-      <c r="O69">
-        <f t="shared" si="16"/>
+      <c r="O74">
+        <f t="shared" si="17"/>
         <v>0.65263751584951402</v>
       </c>
-      <c r="P69">
-        <f t="shared" si="16"/>
+      <c r="P74">
+        <f t="shared" si="17"/>
         <v>0.66629834254143649</v>
       </c>
-      <c r="Q69">
-        <f t="shared" si="16"/>
+      <c r="Q74">
+        <f t="shared" si="17"/>
         <v>0.68950276243093922</v>
       </c>
-      <c r="R69">
-        <f t="shared" si="16"/>
+      <c r="R74">
+        <f t="shared" si="17"/>
         <v>0.71160220994475143</v>
       </c>
-      <c r="S69">
-        <f t="shared" si="16"/>
+      <c r="S74">
+        <f t="shared" si="17"/>
         <v>0.73370165745856375</v>
       </c>
-      <c r="T69">
-        <f t="shared" si="16"/>
+      <c r="T74">
+        <f t="shared" si="17"/>
         <v>0.75580110497237596</v>
       </c>
-      <c r="U69">
-        <f t="shared" si="16"/>
+      <c r="U74">
+        <f t="shared" si="17"/>
         <v>0.77790055248618817</v>
       </c>
-      <c r="V69">
-        <f t="shared" si="16"/>
+      <c r="V74">
+        <f t="shared" si="17"/>
         <v>0.80000000000000027</v>
       </c>
-      <c r="W69">
-        <f t="shared" si="16"/>
+      <c r="W74">
+        <f t="shared" si="17"/>
         <v>0.82209944751381225</v>
       </c>
-      <c r="X69">
-        <f t="shared" si="16"/>
+      <c r="X74">
+        <f t="shared" si="17"/>
         <v>0.84419889502762435</v>
       </c>
-      <c r="Y69">
-        <f t="shared" si="16"/>
+      <c r="Y74">
+        <f t="shared" si="17"/>
         <v>0.86629834254143645</v>
       </c>
-      <c r="Z69">
-        <f t="shared" si="16"/>
+      <c r="Z74">
+        <f t="shared" si="17"/>
         <v>0.88950276243093918</v>
       </c>
-      <c r="AA69">
-        <f t="shared" si="16"/>
+      <c r="AA74">
+        <f t="shared" si="17"/>
         <v>0.91160220994475138</v>
       </c>
-      <c r="AB69">
-        <f t="shared" si="16"/>
+      <c r="AB74">
+        <f t="shared" si="17"/>
         <v>0.93370165745856359</v>
       </c>
-      <c r="AC69">
-        <f t="shared" si="16"/>
+      <c r="AC74">
+        <f t="shared" si="17"/>
         <v>0.95580110497237569</v>
       </c>
-      <c r="AD69">
-        <f t="shared" si="16"/>
+      <c r="AD74">
+        <f t="shared" si="17"/>
         <v>0.9779005524861879</v>
       </c>
-      <c r="AE69">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="C70" t="str">
-        <f>"("&amp;C62&amp;","&amp;ROUND(C68/MAX($C68:$AE68),3)&amp;"),"</f>
+      <c r="AE74">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="C75" t="str">
+        <f>"("&amp;C67&amp;","&amp;ROUND(C73/MAX($C73:$AE73),3)&amp;"),"</f>
         <v>(2022,0.225),</v>
       </c>
-      <c r="D70" t="str">
-        <f t="shared" ref="D70:AE70" si="17">"("&amp;D62&amp;","&amp;ROUND(D68/MAX($C68:$AE68),3)&amp;"),"</f>
+      <c r="D75" t="str">
+        <f t="shared" ref="D75:AE75" si="18">"("&amp;D67&amp;","&amp;ROUND(D73/MAX($C73:$AE73),3)&amp;"),"</f>
         <v>(2023,0.218),</v>
       </c>
-      <c r="E70" t="str">
-        <f t="shared" si="17"/>
+      <c r="E75" t="str">
+        <f t="shared" si="18"/>
         <v>(2024,0.114),</v>
       </c>
-      <c r="F70" t="str">
-        <f t="shared" si="17"/>
-        <v>(2025,0.128),</v>
-      </c>
-      <c r="G70" t="str">
-        <f t="shared" si="17"/>
-        <v>(2026,0.174),</v>
-      </c>
-      <c r="H70" t="str">
-        <f t="shared" si="17"/>
-        <v>(2027,0.235),</v>
-      </c>
-      <c r="I70" t="str">
-        <f t="shared" si="17"/>
+      <c r="F75" t="str">
+        <f t="shared" si="18"/>
+        <v>(2025,0.158),</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="18"/>
+        <v>(2026,0.208),</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="18"/>
+        <v>(2027,0.269),</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="18"/>
         <v>(2028,0.25),</v>
       </c>
-      <c r="J70" t="str">
-        <f t="shared" si="17"/>
+      <c r="J75" t="str">
+        <f t="shared" si="18"/>
         <v>(2029,0.297),</v>
       </c>
-      <c r="K70" t="str">
-        <f t="shared" si="17"/>
+      <c r="K75" t="str">
+        <f t="shared" si="18"/>
         <v>(2030,0.339),</v>
       </c>
-      <c r="L70" t="str">
-        <f t="shared" si="17"/>
+      <c r="L75" t="str">
+        <f t="shared" si="18"/>
         <v>(2031,0.36),</v>
       </c>
-      <c r="M70" t="str">
-        <f t="shared" si="17"/>
+      <c r="M75" t="str">
+        <f t="shared" si="18"/>
         <v>(2032,0.415),</v>
       </c>
-      <c r="N70" t="str">
-        <f t="shared" si="17"/>
+      <c r="N75" t="str">
+        <f t="shared" si="18"/>
         <v>(2033,0.494),</v>
       </c>
-      <c r="O70" t="str">
-        <f t="shared" si="17"/>
+      <c r="O75" t="str">
+        <f t="shared" si="18"/>
         <v>(2034,0.569),</v>
       </c>
-      <c r="P70" t="str">
-        <f t="shared" si="17"/>
+      <c r="P75" t="str">
+        <f t="shared" si="18"/>
         <v>(2035,0.64),</v>
       </c>
-      <c r="Q70" t="str">
-        <f t="shared" si="17"/>
+      <c r="Q75" t="str">
+        <f t="shared" si="18"/>
         <v>(2036,0.707),</v>
       </c>
-      <c r="R70" t="str">
-        <f t="shared" si="17"/>
+      <c r="R75" t="str">
+        <f t="shared" si="18"/>
         <v>(2037,0.771),</v>
       </c>
-      <c r="S70" t="str">
-        <f t="shared" si="17"/>
+      <c r="S75" t="str">
+        <f t="shared" si="18"/>
         <v>(2038,0.832),</v>
       </c>
-      <c r="T70" t="str">
-        <f t="shared" si="17"/>
+      <c r="T75" t="str">
+        <f t="shared" si="18"/>
         <v>(2039,0.889),</v>
       </c>
-      <c r="U70" t="str">
-        <f t="shared" si="17"/>
+      <c r="U75" t="str">
+        <f t="shared" si="18"/>
         <v>(2040,0.943),</v>
       </c>
-      <c r="V70" t="str">
-        <f t="shared" si="17"/>
+      <c r="V75" t="str">
+        <f t="shared" si="18"/>
         <v>(2041,0.958),</v>
       </c>
-      <c r="W70" t="str">
-        <f t="shared" si="17"/>
+      <c r="W75" t="str">
+        <f t="shared" si="18"/>
         <v>(2042,0.971),</v>
       </c>
-      <c r="X70" t="str">
-        <f t="shared" si="17"/>
+      <c r="X75" t="str">
+        <f t="shared" si="18"/>
         <v>(2043,0.982),</v>
       </c>
-      <c r="Y70" t="str">
-        <f t="shared" si="17"/>
+      <c r="Y75" t="str">
+        <f t="shared" si="18"/>
         <v>(2044,0.992),</v>
       </c>
-      <c r="Z70" t="str">
-        <f t="shared" si="17"/>
+      <c r="Z75" t="str">
+        <f t="shared" si="18"/>
         <v>(2045,1),</v>
       </c>
-      <c r="AA70" t="str">
-        <f t="shared" si="17"/>
+      <c r="AA75" t="str">
+        <f t="shared" si="18"/>
         <v>(2046,0.974),</v>
       </c>
-      <c r="AB70" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB75" t="str">
+        <f t="shared" si="18"/>
         <v>(2047,0.948),</v>
       </c>
-      <c r="AC70" t="str">
-        <f t="shared" si="17"/>
+      <c r="AC75" t="str">
+        <f t="shared" si="18"/>
         <v>(2048,0.922),</v>
       </c>
-      <c r="AD70" t="str">
-        <f t="shared" si="17"/>
+      <c r="AD75" t="str">
+        <f t="shared" si="18"/>
         <v>(2049,0.896),</v>
       </c>
-      <c r="AE70" t="str">
-        <f t="shared" si="17"/>
+      <c r="AE75" t="str">
+        <f t="shared" si="18"/>
         <v>(2050,0.87),</v>
       </c>
     </row>
@@ -5996,119 +6061,119 @@
         <v>0</v>
       </c>
       <c r="C3" s="3">
-        <f>'ETS Projections'!C66</f>
+        <f>'ETS Projections'!C71</f>
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <f>'ETS Projections'!D66</f>
+        <f>'ETS Projections'!D71</f>
         <v>0</v>
       </c>
       <c r="E3" s="3">
-        <f>'ETS Projections'!E66</f>
+        <f>'ETS Projections'!E71</f>
         <v>0</v>
       </c>
       <c r="F3" s="3">
-        <f>'ETS Projections'!F66</f>
+        <f>'ETS Projections'!F71</f>
         <v>0</v>
       </c>
       <c r="G3" s="3">
-        <f>'ETS Projections'!G66</f>
+        <f>'ETS Projections'!G71</f>
         <v>0</v>
       </c>
       <c r="H3" s="3">
-        <f>'ETS Projections'!H66</f>
-        <v>0.4825395020511708</v>
+        <f>'ETS Projections'!H71</f>
+        <v>0.45136590456397085</v>
       </c>
       <c r="I3" s="3">
-        <f>'ETS Projections'!I66</f>
+        <f>'ETS Projections'!I71</f>
         <v>0.66393045842516363</v>
       </c>
       <c r="J3" s="3">
-        <f>'ETS Projections'!J66</f>
+        <f>'ETS Projections'!J71</f>
         <v>0.77077996942773064</v>
       </c>
       <c r="K3" s="3">
-        <f>'ETS Projections'!K66</f>
+        <f>'ETS Projections'!K71</f>
         <v>0.85792340111752319</v>
       </c>
       <c r="L3" s="3">
-        <f>'ETS Projections'!L66</f>
+        <f>'ETS Projections'!L71</f>
         <v>0.95998088009684113</v>
       </c>
       <c r="M3" s="3">
-        <f>'ETS Projections'!M66</f>
+        <f>'ETS Projections'!M71</f>
         <v>1</v>
       </c>
       <c r="N3" s="3">
-        <f>'ETS Projections'!N66</f>
+        <f>'ETS Projections'!N71</f>
         <v>1</v>
       </c>
       <c r="O3" s="3">
-        <f>'ETS Projections'!O66</f>
+        <f>'ETS Projections'!O71</f>
         <v>1</v>
       </c>
       <c r="P3" s="3">
-        <f>'ETS Projections'!P66</f>
+        <f>'ETS Projections'!P71</f>
         <v>1</v>
       </c>
       <c r="Q3" s="3">
-        <f>'ETS Projections'!Q66</f>
+        <f>'ETS Projections'!Q71</f>
         <v>1</v>
       </c>
       <c r="R3" s="3">
-        <f>'ETS Projections'!R66</f>
+        <f>'ETS Projections'!R71</f>
         <v>1</v>
       </c>
       <c r="S3" s="3">
-        <f>'ETS Projections'!S66</f>
+        <f>'ETS Projections'!S71</f>
         <v>1</v>
       </c>
       <c r="T3" s="3">
-        <f>'ETS Projections'!T66</f>
+        <f>'ETS Projections'!T71</f>
         <v>1</v>
       </c>
       <c r="U3" s="3">
-        <f>'ETS Projections'!U66</f>
+        <f>'ETS Projections'!U71</f>
         <v>1</v>
       </c>
       <c r="V3" s="3">
-        <f>'ETS Projections'!V66</f>
+        <f>'ETS Projections'!V71</f>
         <v>1</v>
       </c>
       <c r="W3" s="3">
-        <f>'ETS Projections'!W66</f>
+        <f>'ETS Projections'!W71</f>
         <v>1</v>
       </c>
       <c r="X3" s="3">
-        <f>'ETS Projections'!X66</f>
+        <f>'ETS Projections'!X71</f>
         <v>1</v>
       </c>
       <c r="Y3" s="3">
-        <f>'ETS Projections'!Y66</f>
+        <f>'ETS Projections'!Y71</f>
         <v>1</v>
       </c>
       <c r="Z3" s="3">
-        <f>'ETS Projections'!Z66</f>
+        <f>'ETS Projections'!Z71</f>
         <v>1</v>
       </c>
       <c r="AA3" s="3">
-        <f>'ETS Projections'!AA66</f>
+        <f>'ETS Projections'!AA71</f>
         <v>1</v>
       </c>
       <c r="AB3" s="3">
-        <f>'ETS Projections'!AB66</f>
+        <f>'ETS Projections'!AB71</f>
         <v>1</v>
       </c>
       <c r="AC3" s="3">
-        <f>'ETS Projections'!AC66</f>
+        <f>'ETS Projections'!AC71</f>
         <v>1</v>
       </c>
       <c r="AD3" s="3">
-        <f>'ETS Projections'!AD66</f>
+        <f>'ETS Projections'!AD71</f>
         <v>1</v>
       </c>
       <c r="AE3" s="3">
-        <f>'ETS Projections'!AE66</f>
+        <f>'ETS Projections'!AE71</f>
         <v>1</v>
       </c>
     </row>
@@ -6141,7 +6206,7 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" si="0"/>
-        <v>0.4825395020511708</v>
+        <v>0.45136590456397085</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="0"/>
@@ -6245,119 +6310,119 @@
         <v>0.18000000000000005</v>
       </c>
       <c r="C5" s="9">
-        <f>(1-Data!$A3)*'ETS Projections'!C65</f>
+        <f>(1-Data!$A3)*'ETS Projections'!C70</f>
         <v>0.18000000000000005</v>
       </c>
       <c r="D5" s="9">
-        <f>(1-Data!$A3)*'ETS Projections'!D65</f>
+        <f>(1-Data!$A3)*'ETS Projections'!D70</f>
         <v>0.18000000000000005</v>
       </c>
       <c r="E5" s="9">
-        <f>(1-Data!A8)*'ETS Projections'!E65</f>
+        <f>(1-Data!A8)*'ETS Projections'!E70</f>
         <v>0.25</v>
       </c>
       <c r="F5" s="9">
-        <f>(1-Data!A9)*'ETS Projections'!F65</f>
+        <f>(1-Data!A9)*'ETS Projections'!F70</f>
         <v>0.5</v>
       </c>
       <c r="G5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!G65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!G70</f>
         <v>1</v>
       </c>
       <c r="H5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!H65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!H70</f>
         <v>1</v>
       </c>
       <c r="I5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!I65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!I70</f>
         <v>1</v>
       </c>
       <c r="J5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!J65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!J70</f>
         <v>1</v>
       </c>
       <c r="K5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!K65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!K70</f>
         <v>1</v>
       </c>
       <c r="L5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!L65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!L70</f>
         <v>1</v>
       </c>
       <c r="M5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!M65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!M70</f>
         <v>0.91911276045243906</v>
       </c>
       <c r="N5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!N65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!N70</f>
         <v>0.82015499738072961</v>
       </c>
       <c r="O5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!O65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!O70</f>
         <v>0.76702920449344913</v>
       </c>
       <c r="P5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!P65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!P70</f>
         <v>0.71887152156448098</v>
       </c>
       <c r="Q5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!Q65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!Q70</f>
         <v>0.68980453195441105</v>
       </c>
       <c r="R5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!R65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!R70</f>
         <v>0.66563926421639297</v>
       </c>
       <c r="S5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!S65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!S70</f>
         <v>0.64618847711678717</v>
       </c>
       <c r="T5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!T65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!T70</f>
         <v>0.6304675233748841</v>
       </c>
       <c r="U5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!U65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!U70</f>
         <v>0.61775493845911467</v>
       </c>
       <c r="V5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!V65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!V70</f>
         <v>0.62308739476792896</v>
       </c>
       <c r="W5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!W65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!W70</f>
         <v>0.62891664700627326</v>
       </c>
       <c r="X5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!X65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!X70</f>
         <v>0.63521305905982683</v>
       </c>
       <c r="Y5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!Y65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!Y70</f>
         <v>0.641951661578396</v>
       </c>
       <c r="Z5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!Z65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!Z70</f>
         <v>0.64991874023548524</v>
       </c>
       <c r="AA5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!AA65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!AA70</f>
         <v>0.6719213131081081</v>
       </c>
       <c r="AB5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!AB65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!AB70</f>
         <v>0.69434436309455783</v>
       </c>
       <c r="AC5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!AC65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!AC70</f>
         <v>0.71719848448643142</v>
       </c>
       <c r="AD5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!AD65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!AD70</f>
         <v>0.74049442492889994</v>
       </c>
       <c r="AE5" s="9">
-        <f>(1-Data!$A10)*'ETS Projections'!AE65</f>
+        <f>(1-Data!$A10)*'ETS Projections'!AE70</f>
         <v>0.76424309180226624</v>
       </c>
     </row>
@@ -6470,111 +6535,111 @@
         <v>0</v>
       </c>
       <c r="E7" s="9">
-        <f>'ETS Projections'!E65*Data!$A14</f>
+        <f>'ETS Projections'!E70*Data!$A14</f>
         <v>0.4</v>
       </c>
       <c r="F7" s="9">
-        <f>'ETS Projections'!F65*Data!$A15</f>
+        <f>'ETS Projections'!F70*Data!$A15</f>
         <v>0.7</v>
       </c>
       <c r="G7" s="9">
-        <f>'ETS Projections'!G65*Data!$A16</f>
+        <f>'ETS Projections'!G70*Data!$A16</f>
         <v>1</v>
       </c>
       <c r="H7" s="9">
-        <f>'ETS Projections'!H65*Data!$A16</f>
+        <f>'ETS Projections'!H70*Data!$A16</f>
         <v>1</v>
       </c>
       <c r="I7" s="9">
-        <f>'ETS Projections'!I65*Data!$A16</f>
+        <f>'ETS Projections'!I70*Data!$A16</f>
         <v>1</v>
       </c>
       <c r="J7" s="9">
-        <f>'ETS Projections'!J65*Data!$A16</f>
+        <f>'ETS Projections'!J70*Data!$A16</f>
         <v>1</v>
       </c>
       <c r="K7" s="9">
-        <f>'ETS Projections'!K65*Data!$A16</f>
+        <f>'ETS Projections'!K70*Data!$A16</f>
         <v>1</v>
       </c>
       <c r="L7" s="9">
-        <f>'ETS Projections'!L65*Data!$A16</f>
+        <f>'ETS Projections'!L70*Data!$A16</f>
         <v>1</v>
       </c>
       <c r="M7" s="9">
-        <f>'ETS Projections'!M65*Data!$A16</f>
+        <f>'ETS Projections'!M70*Data!$A16</f>
         <v>0.91911276045243906</v>
       </c>
       <c r="N7" s="9">
-        <f>'ETS Projections'!N65*Data!$A16</f>
+        <f>'ETS Projections'!N70*Data!$A16</f>
         <v>0.82015499738072961</v>
       </c>
       <c r="O7" s="9">
-        <f>'ETS Projections'!O65*Data!$A16</f>
+        <f>'ETS Projections'!O70*Data!$A16</f>
         <v>0.76702920449344913</v>
       </c>
       <c r="P7" s="9">
-        <f>'ETS Projections'!P65*Data!$A16</f>
+        <f>'ETS Projections'!P70*Data!$A16</f>
         <v>0.71887152156448098</v>
       </c>
       <c r="Q7" s="9">
-        <f>'ETS Projections'!Q65*Data!$A16</f>
+        <f>'ETS Projections'!Q70*Data!$A16</f>
         <v>0.68980453195441105</v>
       </c>
       <c r="R7" s="9">
-        <f>'ETS Projections'!R65*Data!$A16</f>
+        <f>'ETS Projections'!R70*Data!$A16</f>
         <v>0.66563926421639297</v>
       </c>
       <c r="S7" s="9">
-        <f>'ETS Projections'!S65*Data!$A16</f>
+        <f>'ETS Projections'!S70*Data!$A16</f>
         <v>0.64618847711678717</v>
       </c>
       <c r="T7" s="9">
-        <f>'ETS Projections'!T65*Data!$A16</f>
+        <f>'ETS Projections'!T70*Data!$A16</f>
         <v>0.6304675233748841</v>
       </c>
       <c r="U7" s="9">
-        <f>'ETS Projections'!U65*Data!$A16</f>
+        <f>'ETS Projections'!U70*Data!$A16</f>
         <v>0.61775493845911467</v>
       </c>
       <c r="V7" s="9">
-        <f>'ETS Projections'!V65*Data!$A16</f>
+        <f>'ETS Projections'!V70*Data!$A16</f>
         <v>0.62308739476792896</v>
       </c>
       <c r="W7" s="9">
-        <f>'ETS Projections'!W65*Data!$A16</f>
+        <f>'ETS Projections'!W70*Data!$A16</f>
         <v>0.62891664700627326</v>
       </c>
       <c r="X7" s="9">
-        <f>'ETS Projections'!X65*Data!$A16</f>
+        <f>'ETS Projections'!X70*Data!$A16</f>
         <v>0.63521305905982683</v>
       </c>
       <c r="Y7" s="9">
-        <f>'ETS Projections'!Y65*Data!$A16</f>
+        <f>'ETS Projections'!Y70*Data!$A16</f>
         <v>0.641951661578396</v>
       </c>
       <c r="Z7" s="9">
-        <f>'ETS Projections'!Z65*Data!$A16</f>
+        <f>'ETS Projections'!Z70*Data!$A16</f>
         <v>0.64991874023548524</v>
       </c>
       <c r="AA7" s="9">
-        <f>'ETS Projections'!AA65*Data!$A16</f>
+        <f>'ETS Projections'!AA70*Data!$A16</f>
         <v>0.6719213131081081</v>
       </c>
       <c r="AB7" s="9">
-        <f>'ETS Projections'!AB65*Data!$A16</f>
+        <f>'ETS Projections'!AB70*Data!$A16</f>
         <v>0.69434436309455783</v>
       </c>
       <c r="AC7" s="9">
-        <f>'ETS Projections'!AC65*Data!$A16</f>
+        <f>'ETS Projections'!AC70*Data!$A16</f>
         <v>0.71719848448643142</v>
       </c>
       <c r="AD7" s="9">
-        <f>'ETS Projections'!AD65*Data!$A16</f>
+        <f>'ETS Projections'!AD70*Data!$A16</f>
         <v>0.74049442492889994</v>
       </c>
       <c r="AE7" s="9">
-        <f>'ETS Projections'!AE65*Data!$A16</f>
+        <f>'ETS Projections'!AE70*Data!$A16</f>
         <v>0.76424309180226624</v>
       </c>
     </row>
@@ -6608,7 +6673,7 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>0.4825395020511708</v>
+        <v>0.45136590456397085</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="1"/>
@@ -7463,7 +7528,7 @@
       </c>
       <c r="H2" s="3">
         <f>calcs!H3</f>
-        <v>0.4825395020511708</v>
+        <v>0.45136590456397085</v>
       </c>
       <c r="I2" s="3">
         <f>calcs!I3</f>
@@ -7588,7 +7653,7 @@
       </c>
       <c r="H3" s="3">
         <f>calcs!H4</f>
-        <v>0.4825395020511708</v>
+        <v>0.45136590456397085</v>
       </c>
       <c r="I3" s="3">
         <f>calcs!I4</f>
@@ -8088,7 +8153,7 @@
       </c>
       <c r="H7" s="3">
         <f>calcs!H8</f>
-        <v>0.4825395020511708</v>
+        <v>0.45136590456397085</v>
       </c>
       <c r="I7" s="3">
         <f>calcs!I8</f>

</xml_diff>